<commit_message>
delete and patch ok
</commit_message>
<xml_diff>
--- a/backend/Amet_data_update.xlsx
+++ b/backend/Amet_data_update.xlsx
@@ -540,19 +540,13 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>20-7-23</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>1689856558655</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -591,14 +585,18 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>21-7-23</t>
+        </is>
+      </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>3333333333</v>
+        <v>1689912425716</v>
       </c>
     </row>
     <row r="4">
@@ -644,9 +642,7 @@
       <c r="L4" t="n">
         <v>0</v>
       </c>
-      <c r="M4" t="n">
-        <v>3333333333</v>
-      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -691,9 +687,7 @@
       <c r="L5" t="n">
         <v>0</v>
       </c>
-      <c r="M5" t="n">
-        <v>3333333333</v>
-      </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1740,7 +1734,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1788,6 +1782,150 @@
         <is>
           <t>registerNum</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Shit shit shit</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Rica</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>kuva5008@gmail.com</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>31626117235</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Checking</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>3333333333</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Shit shit shit</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Rica</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>kuva5008@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>31626117235</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Checking</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>3333333333</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Shit shit shit</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Rica</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>kuva5008@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>31626117235</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Checking</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>3333333333</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Infante</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>kuva5008@gmail.com</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>626117235</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Checking the shop</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>1689912425716</v>
       </c>
     </row>
   </sheetData>
@@ -1857,7 +1995,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1907,6 +2045,42 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Burning</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>acrylic / canvas</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>70 x 50 cm</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>600</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>./images/paintings_available/amet-burning.png</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>21-7-23</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>1689912425716</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>